<commit_message>
+ Added document function
</commit_message>
<xml_diff>
--- a/Document/YeuCau.xlsx
+++ b/Document/YeuCau.xlsx
@@ -19,22 +19,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Yêu cầu</t>
   </si>
   <si>
     <t>Nội dung</t>
+  </si>
+  <si>
+    <t>Room Booking System Dataflow Diagram (DFD) FreeProjectz</t>
+  </si>
+  <si>
+    <t>Nhóm</t>
+  </si>
+  <si>
+    <t>Hotel Management</t>
+  </si>
+  <si>
+    <t>Room Management</t>
+  </si>
+  <si>
+    <t>Services Management</t>
+  </si>
+  <si>
+    <t>Payment Management</t>
+  </si>
+  <si>
+    <t>Booking Management</t>
+  </si>
+  <si>
+    <t>Customer Management</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -57,13 +89,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -342,23 +377,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://www.freeprojectz.com/dfd/room-booking-system-dataflow-diagram"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update code Hồ Đình Tuấn + Vũ Hoàng Nam
</commit_message>
<xml_diff>
--- a/Document/YeuCau.xlsx
+++ b/Document/YeuCau.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501C01BB-C47B-487E-9BE1-3CD804B74519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FE91CB-A6EE-4BA3-9C3D-303C337866F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
     <t>Hồ Đình Tuấn + Vũ Hoàng Nam</t>
   </si>
   <si>
-    <t>Nguyễn Tuấn Thành + Thang Văn Diệu Tiến + Nguyễn Xuân Hồng</t>
+    <t>Nguyễn Tuấn Thành + Thang Văn Diệu Tiến + Nguyễn Xuân Hồng.</t>
   </si>
 </sst>
 </file>
@@ -390,7 +390,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>